<commit_message>
added Melissa and Rani
</commit_message>
<xml_diff>
--- a/data/P2P_members_list.xlsx
+++ b/data/P2P_members_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20353"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enrique\Documents\p2p\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enriquemontes/p2p/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C59E430-A029-4D7A-9827-A3782B7B0253}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B2CFA1-46C3-3947-9DF7-D17F691DE127}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="25125" windowHeight="16980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="16980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P2P_members" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="151">
   <si>
     <t>Country</t>
   </si>
@@ -105,15 +105,9 @@
     <t>b.helmuth@northeastern.edu</t>
   </si>
   <si>
-    <t>Cara Estes</t>
-  </si>
-  <si>
     <t>USF</t>
   </si>
   <si>
-    <t>cestes@mail.usf.edu</t>
-  </si>
-  <si>
     <t>Carlos Barboza</t>
   </si>
   <si>
@@ -469,6 +463,21 @@
   </si>
   <si>
     <t>SD</t>
+  </si>
+  <si>
+    <t>Melissa Miner</t>
+  </si>
+  <si>
+    <t>cmminer@ucsc.edu</t>
+  </si>
+  <si>
+    <t>Rani Gaddam</t>
+  </si>
+  <si>
+    <t>gaddam@ucsc.edu</t>
+  </si>
+  <si>
+    <t>[MARINe (UCSC)](https://marine.ucsc.edu/index.html)</t>
   </si>
 </sst>
 </file>
@@ -845,22 +854,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -875,41 +884,41 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" t="s">
         <v>131</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
         <v>132</v>
       </c>
-      <c r="C3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -926,7 +935,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -943,7 +952,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -960,7 +969,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -977,7 +986,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -994,7 +1003,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1011,160 +1020,160 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" t="s">
-        <v>37</v>
       </c>
       <c r="C13" t="s">
         <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="E13" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>114</v>
       </c>
       <c r="C14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>40</v>
       </c>
-      <c r="D14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="B15" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>135</v>
+      </c>
+      <c r="B17" t="s">
+        <v>114</v>
+      </c>
+      <c r="C17" t="s">
         <v>115</v>
       </c>
-      <c r="B15" t="s">
-        <v>116</v>
-      </c>
-      <c r="C15" t="s">
-        <v>117</v>
-      </c>
-      <c r="D15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
+        <v>136</v>
+      </c>
+      <c r="E17" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>48</v>
       </c>
-      <c r="D17" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
+        <v>124</v>
+      </c>
+      <c r="D18" t="s">
+        <v>144</v>
+      </c>
+      <c r="E18" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>137</v>
-      </c>
-      <c r="B18" t="s">
-        <v>116</v>
-      </c>
-      <c r="C18" t="s">
-        <v>117</v>
-      </c>
-      <c r="D18" t="s">
-        <v>138</v>
-      </c>
-      <c r="E18" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>50</v>
       </c>
@@ -1172,426 +1181,443 @@
         <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>126</v>
+        <v>26</v>
       </c>
       <c r="D19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E19" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>52</v>
       </c>
       <c r="B20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" t="s">
         <v>19</v>
       </c>
-      <c r="C20" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" t="s">
-        <v>147</v>
-      </c>
-      <c r="E20" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>58</v>
-      </c>
-      <c r="B22" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" t="s">
-        <v>59</v>
-      </c>
-      <c r="D22" t="s">
-        <v>60</v>
-      </c>
-      <c r="E22" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>62</v>
-      </c>
-      <c r="B23" t="s">
-        <v>63</v>
-      </c>
       <c r="C23" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
       <c r="D23" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="E23" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" t="s">
+        <v>119</v>
+      </c>
+      <c r="E27" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>138</v>
+      </c>
+      <c r="B28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" t="s">
+        <v>124</v>
+      </c>
+      <c r="D28" t="s">
+        <v>144</v>
+      </c>
+      <c r="E28" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E29" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" t="s">
+        <v>87</v>
+      </c>
+      <c r="D30" t="s">
+        <v>119</v>
+      </c>
+      <c r="E30" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>120</v>
+      </c>
+      <c r="B31" t="s">
+        <v>121</v>
+      </c>
+      <c r="C31" t="s">
+        <v>122</v>
+      </c>
+      <c r="D31" t="s">
+        <v>145</v>
+      </c>
+      <c r="E31" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" t="s">
+        <v>29</v>
+      </c>
+      <c r="E32" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>92</v>
+      </c>
+      <c r="B33" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" t="s">
+        <v>93</v>
+      </c>
+      <c r="D33" t="s">
+        <v>58</v>
+      </c>
+      <c r="E33" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>126</v>
+      </c>
+      <c r="B34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" t="s">
+        <v>127</v>
+      </c>
+      <c r="D34" t="s">
+        <v>145</v>
+      </c>
+      <c r="E34" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" t="s">
         <v>66</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C35" t="s">
+        <v>96</v>
+      </c>
+      <c r="D35" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>146</v>
+      </c>
+      <c r="B36" t="s">
         <v>19</v>
       </c>
-      <c r="C24" t="s">
-        <v>27</v>
-      </c>
-      <c r="D24" t="s">
-        <v>21</v>
-      </c>
-      <c r="E24" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>69</v>
-      </c>
-      <c r="B25" t="s">
-        <v>70</v>
-      </c>
-      <c r="C25" t="s">
-        <v>71</v>
-      </c>
-      <c r="D25" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>73</v>
-      </c>
-      <c r="B26" t="s">
-        <v>74</v>
-      </c>
-      <c r="C26" t="s">
-        <v>75</v>
-      </c>
-      <c r="D26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>77</v>
-      </c>
-      <c r="B27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" t="s">
-        <v>78</v>
-      </c>
-      <c r="D27" t="s">
-        <v>31</v>
-      </c>
-      <c r="E27" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>80</v>
-      </c>
-      <c r="B28" t="s">
-        <v>81</v>
-      </c>
-      <c r="C28" t="s">
-        <v>82</v>
-      </c>
-      <c r="D28" t="s">
-        <v>121</v>
-      </c>
-      <c r="E28" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>140</v>
-      </c>
-      <c r="B29" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29" t="s">
-        <v>126</v>
-      </c>
-      <c r="D29" t="s">
-        <v>146</v>
-      </c>
-      <c r="E29" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>84</v>
-      </c>
-      <c r="B30" t="s">
-        <v>85</v>
-      </c>
-      <c r="C30" t="s">
-        <v>86</v>
-      </c>
-      <c r="D30" t="s">
-        <v>60</v>
-      </c>
-      <c r="E30" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>87</v>
-      </c>
-      <c r="B31" t="s">
-        <v>88</v>
-      </c>
-      <c r="C31" t="s">
-        <v>89</v>
-      </c>
-      <c r="D31" t="s">
-        <v>121</v>
-      </c>
-      <c r="E31" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>122</v>
-      </c>
-      <c r="B32" t="s">
-        <v>123</v>
-      </c>
-      <c r="C32" t="s">
-        <v>124</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="C36" t="s">
+        <v>150</v>
+      </c>
+      <c r="D36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" t="s">
         <v>147</v>
       </c>
-      <c r="E32" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>91</v>
-      </c>
-      <c r="B33" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" t="s">
-        <v>92</v>
-      </c>
-      <c r="D33" t="s">
-        <v>31</v>
-      </c>
-      <c r="E33" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>94</v>
-      </c>
-      <c r="B34" t="s">
-        <v>74</v>
-      </c>
-      <c r="C34" t="s">
-        <v>95</v>
-      </c>
-      <c r="D34" t="s">
-        <v>60</v>
-      </c>
-      <c r="E34" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>128</v>
-      </c>
-      <c r="B35" t="s">
-        <v>19</v>
-      </c>
-      <c r="C35" t="s">
-        <v>129</v>
-      </c>
-      <c r="D35" t="s">
-        <v>147</v>
-      </c>
-      <c r="E35" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>97</v>
-      </c>
-      <c r="B36" t="s">
-        <v>68</v>
-      </c>
-      <c r="C36" t="s">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>98</v>
-      </c>
-      <c r="D36" t="s">
-        <v>7</v>
-      </c>
-      <c r="E36" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>100</v>
       </c>
       <c r="B37" t="s">
         <v>5</v>
       </c>
       <c r="C37" t="s">
+        <v>99</v>
+      </c>
+      <c r="D37" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>112</v>
+      </c>
+      <c r="B38" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" t="s">
+        <v>80</v>
+      </c>
+      <c r="D38" t="s">
+        <v>119</v>
+      </c>
+      <c r="E38" t="s">
         <v>101</v>
       </c>
-      <c r="D37" t="s">
-        <v>7</v>
-      </c>
-      <c r="E37" t="s">
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>117</v>
+      </c>
+      <c r="B39" t="s">
+        <v>114</v>
+      </c>
+      <c r="C39" t="s">
+        <v>115</v>
+      </c>
+      <c r="D39" t="s">
+        <v>29</v>
+      </c>
+      <c r="E39" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>114</v>
-      </c>
-      <c r="B38" t="s">
-        <v>81</v>
-      </c>
-      <c r="C38" t="s">
-        <v>82</v>
-      </c>
-      <c r="D38" t="s">
-        <v>121</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="B40" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>119</v>
-      </c>
-      <c r="B39" t="s">
-        <v>116</v>
-      </c>
-      <c r="C39" t="s">
-        <v>117</v>
-      </c>
-      <c r="D39" t="s">
-        <v>31</v>
-      </c>
-      <c r="E39" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>148</v>
+      </c>
+      <c r="B41" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" t="s">
+        <v>150</v>
+      </c>
+      <c r="D41" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>139</v>
+      </c>
+      <c r="B42" t="s">
+        <v>61</v>
+      </c>
+      <c r="C42" t="s">
+        <v>140</v>
+      </c>
+      <c r="D42" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>104</v>
       </c>
-      <c r="B40" t="s">
-        <v>43</v>
-      </c>
-      <c r="C40" t="s">
-        <v>44</v>
-      </c>
-      <c r="D40" t="s">
-        <v>7</v>
-      </c>
-      <c r="E40" t="s">
+      <c r="B43" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>141</v>
-      </c>
-      <c r="B41" t="s">
-        <v>63</v>
-      </c>
-      <c r="C41" t="s">
-        <v>142</v>
-      </c>
-      <c r="D41" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="D43" t="s">
+        <v>144</v>
+      </c>
+      <c r="E43" t="s">
         <v>106</v>
       </c>
-      <c r="B42" t="s">
-        <v>19</v>
-      </c>
-      <c r="C42" t="s">
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>107</v>
       </c>
-      <c r="D42" t="s">
-        <v>146</v>
-      </c>
-      <c r="E42" t="s">
+      <c r="B44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="D44" t="s">
+        <v>29</v>
+      </c>
+      <c r="E44" t="s">
         <v>109</v>
-      </c>
-      <c r="B43" t="s">
-        <v>5</v>
-      </c>
-      <c r="C43" t="s">
-        <v>110</v>
-      </c>
-      <c r="D43" t="s">
-        <v>31</v>
-      </c>
-      <c r="E43" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E30" r:id="rId1" xr:uid="{9BC2434D-B975-4F16-A8A7-BE52CDD525EA}"/>
+    <hyperlink ref="E29" r:id="rId1" xr:uid="{9BC2434D-B975-4F16-A8A7-BE52CDD525EA}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
added SI site and link to Brian
</commit_message>
<xml_diff>
--- a/data/P2P_members_list.xlsx
+++ b/data/P2P_members_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enriquemontes/p2p/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B2CFA1-46C3-3947-9DF7-D17F691DE127}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEFCF721-3615-F340-A4FD-B9E986442249}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="16980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -99,9 +99,6 @@
     <t>Brian Helmuth</t>
   </si>
   <si>
-    <t>Northeastern University</t>
-  </si>
-  <si>
     <t>b.helmuth@northeastern.edu</t>
   </si>
   <si>
@@ -478,6 +475,9 @@
   </si>
   <si>
     <t>[MARINe (UCSC)](https://marine.ucsc.edu/index.html)</t>
+  </si>
+  <si>
+    <t>[Northeastern University](https://helmuthlab.cos.northeastern.edu/)</t>
   </si>
 </sst>
 </file>
@@ -857,7 +857,7 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -869,7 +869,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -886,36 +886,36 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" t="s">
         <v>129</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>130</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
         <v>131</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1011,608 +1011,608 @@
         <v>19</v>
       </c>
       <c r="C9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
         <v>24</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
       <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
         <v>28</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>29</v>
-      </c>
-      <c r="E10" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
         <v>32</v>
-      </c>
-      <c r="D11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
         <v>34</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>35</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" t="s">
         <v>36</v>
-      </c>
-      <c r="D12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
         <v>38</v>
-      </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>112</v>
+      </c>
+      <c r="B14" t="s">
         <v>113</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>114</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" t="s">
         <v>115</v>
-      </c>
-      <c r="D14" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
         <v>40</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>41</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
         <v>42</v>
-      </c>
-      <c r="D15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
         <v>44</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>45</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" t="s">
         <v>46</v>
-      </c>
-      <c r="D16" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>134</v>
+      </c>
+      <c r="B17" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17" t="s">
+        <v>114</v>
+      </c>
+      <c r="D17" t="s">
         <v>135</v>
       </c>
-      <c r="B17" t="s">
-        <v>114</v>
-      </c>
-      <c r="C17" t="s">
-        <v>115</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>136</v>
-      </c>
-      <c r="E17" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B19" t="s">
         <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" t="s">
         <v>52</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>53</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" t="s">
         <v>54</v>
-      </c>
-      <c r="D20" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" t="s">
         <v>56</v>
       </c>
-      <c r="B21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>57</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>58</v>
-      </c>
-      <c r="E21" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" t="s">
         <v>60</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>61</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" t="s">
         <v>62</v>
-      </c>
-      <c r="D22" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B23" t="s">
         <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D23" t="s">
         <v>21</v>
       </c>
       <c r="E23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" t="s">
         <v>67</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>68</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" t="s">
         <v>69</v>
-      </c>
-      <c r="D24" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" t="s">
         <v>71</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>72</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" t="s">
         <v>73</v>
-      </c>
-      <c r="D25" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
       </c>
       <c r="C26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" t="s">
         <v>76</v>
-      </c>
-      <c r="D26" t="s">
-        <v>29</v>
-      </c>
-      <c r="E26" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" t="s">
         <v>78</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>79</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
+        <v>118</v>
+      </c>
+      <c r="E27" t="s">
         <v>80</v>
-      </c>
-      <c r="D27" t="s">
-        <v>119</v>
-      </c>
-      <c r="E27" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B28" t="s">
         <v>19</v>
       </c>
       <c r="C28" t="s">
+        <v>123</v>
+      </c>
+      <c r="D28" t="s">
+        <v>143</v>
+      </c>
+      <c r="E28" t="s">
         <v>124</v>
-      </c>
-      <c r="D28" t="s">
-        <v>144</v>
-      </c>
-      <c r="E28" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" t="s">
         <v>82</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>83</v>
       </c>
-      <c r="C29" t="s">
-        <v>84</v>
-      </c>
       <c r="D29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E29" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" t="s">
         <v>85</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>86</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
+        <v>118</v>
+      </c>
+      <c r="E30" t="s">
         <v>87</v>
-      </c>
-      <c r="D30" t="s">
-        <v>119</v>
-      </c>
-      <c r="E30" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>119</v>
+      </c>
+      <c r="B31" t="s">
         <v>120</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>121</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
+        <v>144</v>
+      </c>
+      <c r="E31" t="s">
         <v>122</v>
-      </c>
-      <c r="D31" t="s">
-        <v>145</v>
-      </c>
-      <c r="E31" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B32" t="s">
         <v>5</v>
       </c>
       <c r="C32" t="s">
+        <v>89</v>
+      </c>
+      <c r="D32" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" t="s">
         <v>90</v>
-      </c>
-      <c r="D32" t="s">
-        <v>29</v>
-      </c>
-      <c r="E32" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>91</v>
+      </c>
+      <c r="B33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" t="s">
         <v>92</v>
       </c>
-      <c r="B33" t="s">
-        <v>72</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
+        <v>57</v>
+      </c>
+      <c r="E33" t="s">
         <v>93</v>
-      </c>
-      <c r="D33" t="s">
-        <v>58</v>
-      </c>
-      <c r="E33" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B34" t="s">
         <v>19</v>
       </c>
       <c r="C34" t="s">
+        <v>126</v>
+      </c>
+      <c r="D34" t="s">
+        <v>144</v>
+      </c>
+      <c r="E34" t="s">
         <v>127</v>
-      </c>
-      <c r="D34" t="s">
-        <v>145</v>
-      </c>
-      <c r="E34" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>94</v>
+      </c>
+      <c r="B35" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" t="s">
         <v>95</v>
       </c>
-      <c r="B35" t="s">
-        <v>66</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" t="s">
         <v>96</v>
-      </c>
-      <c r="D35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E35" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B36" t="s">
         <v>19</v>
       </c>
       <c r="C36" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D36" t="s">
         <v>7</v>
       </c>
       <c r="E36" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B37" t="s">
         <v>5</v>
       </c>
       <c r="C37" t="s">
+        <v>98</v>
+      </c>
+      <c r="D37" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" t="s">
         <v>99</v>
-      </c>
-      <c r="D37" t="s">
-        <v>7</v>
-      </c>
-      <c r="E37" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B38" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" t="s">
         <v>79</v>
       </c>
-      <c r="C38" t="s">
-        <v>80</v>
-      </c>
       <c r="D38" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>116</v>
+      </c>
+      <c r="B39" t="s">
+        <v>113</v>
+      </c>
+      <c r="C39" t="s">
+        <v>114</v>
+      </c>
+      <c r="D39" t="s">
+        <v>28</v>
+      </c>
+      <c r="E39" t="s">
         <v>117</v>
-      </c>
-      <c r="B39" t="s">
-        <v>114</v>
-      </c>
-      <c r="C39" t="s">
-        <v>115</v>
-      </c>
-      <c r="D39" t="s">
-        <v>29</v>
-      </c>
-      <c r="E39" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>101</v>
+      </c>
+      <c r="B40" t="s">
+        <v>40</v>
+      </c>
+      <c r="C40" t="s">
+        <v>41</v>
+      </c>
+      <c r="D40" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" t="s">
         <v>102</v>
-      </c>
-      <c r="B40" t="s">
-        <v>41</v>
-      </c>
-      <c r="C40" t="s">
-        <v>42</v>
-      </c>
-      <c r="D40" t="s">
-        <v>7</v>
-      </c>
-      <c r="E40" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B41" t="s">
         <v>19</v>
       </c>
       <c r="C41" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D41" t="s">
         <v>7</v>
       </c>
       <c r="E41" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>138</v>
+      </c>
+      <c r="B42" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" t="s">
         <v>139</v>
       </c>
-      <c r="B42" t="s">
-        <v>61</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" t="s">
         <v>140</v>
-      </c>
-      <c r="D42" t="s">
-        <v>7</v>
-      </c>
-      <c r="E42" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B43" t="s">
         <v>19</v>
       </c>
       <c r="C43" t="s">
+        <v>104</v>
+      </c>
+      <c r="D43" t="s">
+        <v>143</v>
+      </c>
+      <c r="E43" t="s">
         <v>105</v>
-      </c>
-      <c r="D43" t="s">
-        <v>144</v>
-      </c>
-      <c r="E43" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B44" t="s">
         <v>5</v>
       </c>
       <c r="C44" t="s">
+        <v>107</v>
+      </c>
+      <c r="D44" t="s">
+        <v>28</v>
+      </c>
+      <c r="E44" t="s">
         <v>108</v>
-      </c>
-      <c r="D44" t="s">
-        <v>29</v>
-      </c>
-      <c r="E44" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added photos and links to collabs
</commit_message>
<xml_diff>
--- a/data/P2P_members_list.xlsx
+++ b/data/P2P_members_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enriquemontes/p2p/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEFCF721-3615-F340-A4FD-B9E986442249}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05503762-7080-A14E-9E2C-9927B1836750}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="16980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="340" yWindow="2840" windowWidth="33460" windowHeight="14980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P2P_members" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="149">
   <si>
     <t>Country</t>
   </si>
@@ -39,114 +39,57 @@
     <t>email</t>
   </si>
   <si>
-    <t>Ana Carolina Mazzuco</t>
-  </si>
-  <si>
     <t>Brazil</t>
   </si>
   <si>
-    <t>Universidade Federal do Espirito Santo</t>
-  </si>
-  <si>
     <t>RS</t>
   </si>
   <si>
     <t>ac.mazzuco@me.com</t>
   </si>
   <si>
-    <t>Andrew Cooper</t>
-  </si>
-  <si>
     <t>Canada</t>
   </si>
   <si>
-    <t>DFO</t>
-  </si>
-  <si>
     <t>Andrew.Cooper@dfo-mpo.gc.ca</t>
   </si>
   <si>
-    <t>Antonio Marques</t>
-  </si>
-  <si>
-    <t>CEBIMar</t>
-  </si>
-  <si>
     <t>marques@ib.usp.br</t>
   </si>
   <si>
-    <t>Augusto Flores</t>
-  </si>
-  <si>
     <t>guca@usp.br</t>
   </si>
   <si>
-    <t>Ben Best</t>
-  </si>
-  <si>
     <t>USA</t>
   </si>
   <si>
-    <t>EcoQuants</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
     <t>ben@ecoquants.com</t>
   </si>
   <si>
-    <t>Brian Helmuth</t>
-  </si>
-  <si>
     <t>b.helmuth@northeastern.edu</t>
   </si>
   <si>
-    <t>USF</t>
-  </si>
-  <si>
     <t>Carlos Barboza</t>
   </si>
   <si>
-    <t>Universidade Federal do Rio de Janeiro - NUPEM</t>
-  </si>
-  <si>
     <t>SB</t>
   </si>
   <si>
     <t>carlosambarboza@gmail.com</t>
   </si>
   <si>
-    <t>Cesar Cordeiro</t>
-  </si>
-  <si>
-    <t>Universidade Federal Fluminense</t>
-  </si>
-  <si>
     <t>cammcordeiro@gmail.com</t>
   </si>
   <si>
-    <t>Daniela Yepes</t>
-  </si>
-  <si>
     <t>Colombia</t>
   </si>
   <si>
-    <t>INVEMAR</t>
-  </si>
-  <si>
-    <t>daniela.yepes@invemar.org.co</t>
-  </si>
-  <si>
-    <t>Universidad del Valle</t>
-  </si>
-  <si>
     <t>edgardo.londono@correounivalle.edu.co</t>
   </si>
   <si>
-    <t>Eduardo Klein</t>
-  </si>
-  <si>
     <t>Australia</t>
   </si>
   <si>
@@ -156,78 +99,42 @@
     <t>eklein@usb.ve</t>
   </si>
   <si>
-    <t>Eleonora Celentano</t>
-  </si>
-  <si>
     <t>Uruguay</t>
   </si>
   <si>
-    <t>UNDECIMAR - U. de la Rep.</t>
-  </si>
-  <si>
     <t>ecelentano@gmail.com</t>
   </si>
   <si>
-    <t>Emmett Duffy</t>
-  </si>
-  <si>
     <t>DuffyE@si.edu</t>
   </si>
   <si>
-    <t>Enrique Montes</t>
-  </si>
-  <si>
     <t>emontesh@mail.usf.edu</t>
   </si>
   <si>
-    <t>Erasmo Macaya</t>
-  </si>
-  <si>
     <t>Chile</t>
   </si>
   <si>
-    <t>U. Concepcion</t>
-  </si>
-  <si>
     <t>emacaya@oceanografia.udec.cl</t>
   </si>
   <si>
-    <t>Eulogio Soto</t>
-  </si>
-  <si>
-    <t>U. Valparaiso</t>
-  </si>
-  <si>
     <t>RS &amp; SB</t>
   </si>
   <si>
     <t>eulogio.soto@uv.cl</t>
   </si>
   <si>
-    <t>Fernando Lima</t>
-  </si>
-  <si>
     <t>Portugal</t>
   </si>
   <si>
-    <t>University of Porto</t>
-  </si>
-  <si>
     <t>fplima@gmail.com</t>
   </si>
   <si>
-    <t>Frank Muller-Karger</t>
-  </si>
-  <si>
     <t>carib@usf.edu</t>
   </si>
   <si>
     <t>Ecuador</t>
   </si>
   <si>
-    <t>Gil Rilov</t>
-  </si>
-  <si>
     <t>Israel</t>
   </si>
   <si>
@@ -237,15 +144,9 @@
     <t>rilovg@ocean.org.il</t>
   </si>
   <si>
-    <t>Gregorio Bigatti</t>
-  </si>
-  <si>
     <t>Argentina</t>
   </si>
   <si>
-    <t>IBIOMAR-CONICET</t>
-  </si>
-  <si>
     <t>gbigatti@cenpat-conicet.gob.ar</t>
   </si>
   <si>
@@ -258,126 +159,60 @@
     <t>guilhermecorte@yahoo.com.br</t>
   </si>
   <si>
-    <t>Inti Keith</t>
-  </si>
-  <si>
     <t>Ecuador - Galapagos</t>
   </si>
   <si>
-    <t>Charles Darwin Foundation</t>
-  </si>
-  <si>
     <t>inti.keith@fcdarwin.org.ec</t>
   </si>
   <si>
-    <t>Juan Azofeifa</t>
-  </si>
-  <si>
     <t>Costa Rica</t>
   </si>
   <si>
-    <t>CIMAR - Universidad de Costa Rica</t>
-  </si>
-  <si>
     <t>Kristin Wilson Grimes</t>
   </si>
   <si>
     <t>US VI</t>
   </si>
   <si>
-    <t>U. Virgin Islands</t>
-  </si>
-  <si>
     <t>kristin.wilson@uvi.edu</t>
   </si>
   <si>
-    <t>Maikon Di Domenico</t>
-  </si>
-  <si>
-    <t>Universidade Federal do Paranˆ</t>
-  </si>
-  <si>
     <t>maik2dd@gmail.com</t>
   </si>
   <si>
-    <t>Maria Gabriela Palomo</t>
-  </si>
-  <si>
-    <t>Museo Argentino de Ciencias Naturales</t>
-  </si>
-  <si>
     <t>gabi.palomo@hotmail.com</t>
   </si>
   <si>
-    <t>Maritza Cardenas</t>
-  </si>
-  <si>
-    <t>Universidad de Guayaquil</t>
-  </si>
-  <si>
     <t>maritzacardenas@hotmail.com</t>
   </si>
   <si>
-    <t>Moyses Barbosa</t>
-  </si>
-  <si>
-    <t>Universidade Federal Fluminese</t>
-  </si>
-  <si>
-    <t>moyses_barbosa@yahoo.com.br</t>
-  </si>
-  <si>
     <t>nicolas.moity@fcdarwin.org.ec</t>
   </si>
   <si>
-    <t>Patricia Miloslavich</t>
-  </si>
-  <si>
     <t>pmilos@usb.ve</t>
   </si>
   <si>
     <t>Sennai Habtes</t>
   </si>
   <si>
-    <t>UVI</t>
-  </si>
-  <si>
     <t>sennai.habtes@uvi.edu</t>
   </si>
   <si>
-    <t>Yasmina Shah Esmaeili</t>
-  </si>
-  <si>
     <t>Universidade Estadual de Campinas</t>
   </si>
   <si>
     <t>yasmina.shahesmaeili@gmail.com</t>
   </si>
   <si>
-    <t>Edgardo Londoño</t>
-  </si>
-  <si>
     <t>MEMBERS</t>
   </si>
   <si>
-    <t>Nicolas Moity</t>
-  </si>
-  <si>
-    <t>Edlin Guerra</t>
-  </si>
-  <si>
     <t>Mexico</t>
   </si>
   <si>
-    <t>Universidad Nacional Autonoma de Mexico</t>
-  </si>
-  <si>
     <t xml:space="preserve">edlin.guerra@enesmerida.unam.mx </t>
   </si>
   <si>
-    <t>Nuno Simoes</t>
-  </si>
-  <si>
     <t xml:space="preserve">ns@ciencias.unam.mx </t>
   </si>
   <si>
@@ -390,24 +225,12 @@
     <t>Peru</t>
   </si>
   <si>
-    <t>IMARPE</t>
-  </si>
-  <si>
     <t xml:space="preserve">lescudero@imarpe.gob.pe </t>
   </si>
   <si>
-    <t>MarineGEO - Smithsonian I.</t>
-  </si>
-  <si>
     <t xml:space="preserve">LefcheckJ@si.edu </t>
   </si>
   <si>
-    <t>Maria Kavanaugh</t>
-  </si>
-  <si>
-    <t>Oregon State University</t>
-  </si>
-  <si>
     <t xml:space="preserve">mkavanau@ceoas.oregonstate.edu </t>
   </si>
   <si>
@@ -417,36 +240,15 @@
     <t>Trinidad &amp; Tobago</t>
   </si>
   <si>
-    <t>University of West Indies</t>
-  </si>
-  <si>
     <t xml:space="preserve">alana.jute@gmail.com </t>
   </si>
   <si>
-    <t>Abigail Benson</t>
-  </si>
-  <si>
-    <t>OBIS-USA / USGS</t>
-  </si>
-  <si>
-    <t>Elva Escobar-Briones</t>
-  </si>
-  <si>
     <t>Deep sea</t>
   </si>
   <si>
     <t>escobri@cmarl.unam.mx</t>
   </si>
   <si>
-    <t>Jonathan Lefcheck</t>
-  </si>
-  <si>
-    <t>Rui Seabra</t>
-  </si>
-  <si>
-    <t>U. Porto</t>
-  </si>
-  <si>
     <t xml:space="preserve">ruisea@gmail.com </t>
   </si>
   <si>
@@ -478,6 +280,198 @@
   </si>
   <si>
     <t>[Northeastern University](https://helmuthlab.cos.northeastern.edu/)</t>
+  </si>
+  <si>
+    <t>[Maritza Cardenas](https://oceanexpert.org/expert/30409)</t>
+  </si>
+  <si>
+    <t>[Abigail Benson](https://oceanexpert.org/expert/25483)</t>
+  </si>
+  <si>
+    <t>[Ana Carolina Mazzuco](https://oceanexpert.org/expert/34916)</t>
+  </si>
+  <si>
+    <t>[Antonio Marques](https://oceanexpert.org/expert/28123)</t>
+  </si>
+  <si>
+    <t>[Ben Best](https://oceanexpert.org/expert/32717)</t>
+  </si>
+  <si>
+    <t>[Brian Helmuth](https://oceanexpert.org/expert/34874)</t>
+  </si>
+  <si>
+    <t>[Cesar Cordeiro](https://oceanexpert.org/expert/37067)</t>
+  </si>
+  <si>
+    <t>[Edgardo Londoño](https://oceanexpert.org/expert/ELC521)</t>
+  </si>
+  <si>
+    <t>[Edlin Guerra](https://oceanexpert.org/expert/29130)</t>
+  </si>
+  <si>
+    <t>[Eduardo Klein](https://oceanexpert.org/expert/9199)</t>
+  </si>
+  <si>
+    <t>[Eleonora Celentano](https://oceanexpert.org/expert/35001)</t>
+  </si>
+  <si>
+    <t>[Emmett Duffy](https://oceanexpert.org/expert/26366)</t>
+  </si>
+  <si>
+    <t>[Enrique Montes](https://oceanexpert.org/expert/27702)</t>
+  </si>
+  <si>
+    <t>[Erasmo Macaya](https://oceanexpert.org/expert/34965)</t>
+  </si>
+  <si>
+    <t>[Eulogio Soto](https://oceanexpert.org/expert/27487)</t>
+  </si>
+  <si>
+    <t>[Fernando Lima](https://oceanexpert.org/expert/34873)</t>
+  </si>
+  <si>
+    <t>[Frank Muller-Karger](https://oceanexpert.org/expert/1486)</t>
+  </si>
+  <si>
+    <t>[Gil Rilov](https://oceanexpert.org/expert/32405)</t>
+  </si>
+  <si>
+    <t>[Gregorio Bigatti](https://oceanexpert.org/expert/34980)</t>
+  </si>
+  <si>
+    <t>[Inti Keith](https://oceanexpert.org/expert/29486)</t>
+  </si>
+  <si>
+    <t>[Jonathan Lefcheck](https://oceanexpert.org/expert/37241)</t>
+  </si>
+  <si>
+    <t>[Juan Azofeifa](https://oceanexpert.org/expert/34929)</t>
+  </si>
+  <si>
+    <t>[Maikon Di Domenico](https://oceanexpert.org/expert/34925)</t>
+  </si>
+  <si>
+    <t>[Maria Gabriela Palomo](https://oceanexpert.org/expert/29808)</t>
+  </si>
+  <si>
+    <t>[Nicolas Moity](https://oceanexpert.org/expert/29466)</t>
+  </si>
+  <si>
+    <t>[Patricia Miloslavich](https://oceanexpert.org/expert/21855)</t>
+  </si>
+  <si>
+    <t>[Nuno Simoes](https://oceanexpert.org/expert/29123)</t>
+  </si>
+  <si>
+    <t>[Rui Seabra](https://oceanexpert.org/expert/36999)</t>
+  </si>
+  <si>
+    <t>[Yasmina Shah Esmaeili](https://oceanexpert.org/expert/35244)</t>
+  </si>
+  <si>
+    <t>[Gabrielle Canonico](https://oceanexpert.org/expert/27507)</t>
+  </si>
+  <si>
+    <t>[NOAA - IOOS](https://ioos.noaa.gov/)</t>
+  </si>
+  <si>
+    <t>[OBIS-USA / USGS](https://www.usgs.gov/core-science-systems/science-analytics-and-synthesis/obis-usa)</t>
+  </si>
+  <si>
+    <t>[U. West Indies](https://sta.uwi.edu/fst/lifesciences/)</t>
+  </si>
+  <si>
+    <t>[Bentos - UFES](http://bentos.ufes.br/)</t>
+  </si>
+  <si>
+    <t>[CEBIMAR - USP](http://npbiomar.cebimar.usp.br/en/)</t>
+  </si>
+  <si>
+    <t>[EcoQuants](https://ecoquants.com/)</t>
+  </si>
+  <si>
+    <t>[NUPEM - UFRJ](https://www.macae.ufrj.br/nupem/index.php)</t>
+  </si>
+  <si>
+    <t>[LECAR - UFF](http://www.lecar.uff.br/index.html)</t>
+  </si>
+  <si>
+    <t>[U. del Valle](https://lithos.correounivalle.edu.co/)</t>
+  </si>
+  <si>
+    <t>[UNAM](https://www.bdmy.org.mx/)</t>
+  </si>
+  <si>
+    <t>[UNDECIMAR](http://undecimar.fcien.edu.uy/es_ES/)</t>
+  </si>
+  <si>
+    <t>[Elva Escobar-Briones](https://www.icmyl.unam.mx/en/node/4)</t>
+  </si>
+  <si>
+    <t>[ICMyL - UNAM](http://www.icmyl.unam.mx/)</t>
+  </si>
+  <si>
+    <t>[MarineGEO - Smithsonian I.](https://marinegeo.si.edu/)</t>
+  </si>
+  <si>
+    <t>[IMaRS - USF](http://imars.usf.edu/)</t>
+  </si>
+  <si>
+    <t>[U. Concepcion](https://www.algalab.com/index2.html)</t>
+  </si>
+  <si>
+    <t>[U. Valparaiso](https://cienciasdelmar.uv.cl/index.php)</t>
+  </si>
+  <si>
+    <t>[CIBIO - University of Porto](https://cibio.up.pt/research-groups-1/details/marchange)</t>
+  </si>
+  <si>
+    <t>[CMES - UVI](https://www.uvi.edu/research/center-for-marine-environmental-studies/about-cmes/default.aspx)</t>
+  </si>
+  <si>
+    <t>[SCOR](https://scor-int.org/)</t>
+  </si>
+  <si>
+    <t>[Charles Darwin F.](https://www.darwinfoundation.org/en/)</t>
+  </si>
+  <si>
+    <t>[RIEAE - U. Guayaquil](https://www.facebook.com/RED-RIEAE-107397151044316)</t>
+  </si>
+  <si>
+    <t>[CEOAS - OSU[(https://ceoas.oregonstate.edu/)</t>
+  </si>
+  <si>
+    <t>[MACN](https://www.macnconicet.gob.ar/investigacion/ecologia/)</t>
+  </si>
+  <si>
+    <t>[PGSISCO - UFPR](http://www.cem.ufpr.br/portal/pgsisco/selecao-discente/)</t>
+  </si>
+  <si>
+    <t>[IMARPE](http://www.imarpe.gob.pe/imarpe/)</t>
+  </si>
+  <si>
+    <t>[CIMAR](http://www.cimar.ucr.ac.cr/index.php)</t>
+  </si>
+  <si>
+    <t>[IBIOMAR/CONICET](https://www.larbim.com.ar/)</t>
+  </si>
+  <si>
+    <t>Program manager</t>
+  </si>
+  <si>
+    <t>gabrielle.canonico@noaa.gov</t>
+  </si>
+  <si>
+    <t>[DFO](https://profils-profiles.science.gc.ca/en/research-centre/st-andrews-biological-station)</t>
+  </si>
+  <si>
+    <t>[Andrew Cooper](https://profils-profiles.science.gc.ca/en/profile/andrew-cooper)</t>
+  </si>
+  <si>
+    <t>[Augusto Flores](http://cebimar.usp.br/pt/quem-somos/equipe-academica)</t>
+  </si>
+  <si>
+    <t>[Maria Kavanaugh](https://oceanexpert.org/expert/32651)</t>
   </si>
 </sst>
 </file>
@@ -854,22 +848,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>110</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -886,614 +880,614 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="D2" t="s">
-        <v>142</v>
+        <v>76</v>
       </c>
       <c r="E2" t="s">
-        <v>131</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>129</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>131</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
       <c r="C4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
         <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>146</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>145</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>88</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>119</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>147</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>119</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>89</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>90</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>150</v>
+        <v>84</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>121</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>91</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>122</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>92</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>123</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>124</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E13" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="B14" t="s">
-        <v>113</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>114</v>
+        <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="E14" t="s">
-        <v>115</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>95</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>125</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E15" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>126</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>127</v>
       </c>
       <c r="D16" t="s">
-        <v>28</v>
+        <v>72</v>
       </c>
       <c r="E16" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>134</v>
+        <v>96</v>
       </c>
       <c r="B17" t="s">
-        <v>113</v>
+        <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="D17" t="s">
-        <v>135</v>
+        <v>77</v>
       </c>
       <c r="E17" t="s">
-        <v>136</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>97</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="D18" t="s">
-        <v>143</v>
+        <v>78</v>
       </c>
       <c r="E18" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>98</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>25</v>
+        <v>130</v>
       </c>
       <c r="D19" t="s">
-        <v>144</v>
+        <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>99</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>53</v>
+        <v>131</v>
       </c>
       <c r="D20" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="E20" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>100</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>132</v>
       </c>
       <c r="D21" t="s">
-        <v>57</v>
+        <v>5</v>
       </c>
       <c r="E21" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>101</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>129</v>
       </c>
       <c r="D22" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E22" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>114</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C23" t="s">
-        <v>25</v>
+        <v>115</v>
       </c>
       <c r="D23" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
       <c r="E23" t="s">
-        <v>64</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="B24" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="C24" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="D24" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E24" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
       <c r="B25" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="C25" t="s">
-        <v>72</v>
+        <v>142</v>
       </c>
       <c r="D25" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E25" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="B26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="D26" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E26" t="s">
-        <v>76</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>77</v>
+        <v>104</v>
       </c>
       <c r="B27" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="C27" t="s">
-        <v>79</v>
+        <v>135</v>
       </c>
       <c r="D27" t="s">
-        <v>118</v>
+        <v>63</v>
       </c>
       <c r="E27" t="s">
-        <v>80</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="B28" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C28" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="D28" t="s">
-        <v>143</v>
+        <v>77</v>
       </c>
       <c r="E28" t="s">
-        <v>124</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="B29" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="C29" t="s">
-        <v>83</v>
+        <v>141</v>
       </c>
       <c r="D29" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="E29" t="s">
-        <v>141</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>47</v>
       </c>
       <c r="B30" t="s">
-        <v>85</v>
+        <v>48</v>
       </c>
       <c r="C30" t="s">
-        <v>86</v>
+        <v>133</v>
       </c>
       <c r="D30" t="s">
-        <v>118</v>
+        <v>63</v>
       </c>
       <c r="E30" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>119</v>
+        <v>64</v>
       </c>
       <c r="B31" t="s">
-        <v>120</v>
+        <v>65</v>
       </c>
       <c r="C31" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="D31" t="s">
-        <v>144</v>
+        <v>78</v>
       </c>
       <c r="E31" t="s">
-        <v>122</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>88</v>
+        <v>107</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>89</v>
+        <v>139</v>
       </c>
       <c r="D32" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E32" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="B33" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="C33" t="s">
-        <v>92</v>
+        <v>138</v>
       </c>
       <c r="D33" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="E33" t="s">
-        <v>93</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="B34" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="D34" t="s">
-        <v>144</v>
+        <v>78</v>
       </c>
       <c r="E34" t="s">
-        <v>127</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B35" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="C35" t="s">
-        <v>95</v>
+        <v>136</v>
       </c>
       <c r="D35" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E35" t="s">
-        <v>96</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>145</v>
+        <v>79</v>
       </c>
       <c r="B36" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C36" t="s">
-        <v>149</v>
+        <v>83</v>
       </c>
       <c r="D36" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E36" t="s">
-        <v>146</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="B37" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="C37" t="s">
-        <v>98</v>
+        <v>135</v>
       </c>
       <c r="D37" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="E37" t="s">
-        <v>99</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -1501,118 +1495,101 @@
         <v>111</v>
       </c>
       <c r="B38" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="C38" t="s">
-        <v>79</v>
+        <v>124</v>
       </c>
       <c r="D38" t="s">
-        <v>118</v>
+        <v>16</v>
       </c>
       <c r="E38" t="s">
-        <v>100</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B39" t="s">
-        <v>113</v>
+        <v>21</v>
       </c>
       <c r="C39" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
       <c r="D39" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="E39" t="s">
-        <v>117</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="B40" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="C40" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="D40" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E40" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>147</v>
+        <v>112</v>
       </c>
       <c r="B41" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="C41" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="D41" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E41" t="s">
-        <v>148</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>138</v>
+        <v>55</v>
       </c>
       <c r="B42" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C42" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D42" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="E42" t="s">
-        <v>140</v>
+        <v>56</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="B43" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>104</v>
+        <v>57</v>
       </c>
       <c r="D43" t="s">
-        <v>143</v>
+        <v>16</v>
       </c>
       <c r="E43" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>106</v>
-      </c>
-      <c r="B44" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" t="s">
-        <v>107</v>
-      </c>
-      <c r="D44" t="s">
-        <v>28</v>
-      </c>
-      <c r="E44" t="s">
-        <v>108</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected MTK link and added Yas link
</commit_message>
<xml_diff>
--- a/data/P2P_members_list.xlsx
+++ b/data/P2P_members_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enriquemontes/p2p/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05503762-7080-A14E-9E2C-9927B1836750}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD164424-1CB2-BE47-AC2E-D98C8C564EB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="2840" windowWidth="33460" windowHeight="14980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -198,9 +198,6 @@
     <t>sennai.habtes@uvi.edu</t>
   </si>
   <si>
-    <t>Universidade Estadual de Campinas</t>
-  </si>
-  <si>
     <t>yasmina.shahesmaeili@gmail.com</t>
   </si>
   <si>
@@ -219,9 +216,6 @@
     <t>RS/SB</t>
   </si>
   <si>
-    <t>Luis Escudero</t>
-  </si>
-  <si>
     <t>Peru</t>
   </si>
   <si>
@@ -438,9 +432,6 @@
     <t>[RIEAE - U. Guayaquil](https://www.facebook.com/RED-RIEAE-107397151044316)</t>
   </si>
   <si>
-    <t>[CEOAS - OSU[(https://ceoas.oregonstate.edu/)</t>
-  </si>
-  <si>
     <t>[MACN](https://www.macnconicet.gob.ar/investigacion/ecologia/)</t>
   </si>
   <si>
@@ -472,6 +463,15 @@
   </si>
   <si>
     <t>[Maria Kavanaugh](https://oceanexpert.org/expert/32651)</t>
+  </si>
+  <si>
+    <t>[CEOAS - OSU](https://ceoas.oregonstate.edu/)</t>
+  </si>
+  <si>
+    <t>[UNICAMP](https://www.ib.unicamp.br/)</t>
+  </si>
+  <si>
+    <t>[Luis Escudero](https://www.gob.pe/institucion/imarpe/funcionarios/30904-luis-orlando-escudero-herrera)</t>
   </si>
 </sst>
 </file>
@@ -850,8 +850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -863,7 +863,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -880,47 +880,47 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
         <v>69</v>
-      </c>
-      <c r="B3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -931,13 +931,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
@@ -948,13 +948,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
@@ -965,13 +965,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
@@ -982,13 +982,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
@@ -999,13 +999,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
@@ -1022,7 +1022,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D10" t="s">
         <v>16</v>
@@ -1033,13 +1033,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D11" t="s">
         <v>5</v>
@@ -1050,13 +1050,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B12" t="s">
         <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>
@@ -1067,24 +1067,24 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D13" t="s">
         <v>16</v>
       </c>
       <c r="E13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B14" t="s">
         <v>21</v>
@@ -1101,13 +1101,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B15" t="s">
         <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D15" t="s">
         <v>16</v>
@@ -1118,33 +1118,33 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E17" t="s">
         <v>26</v>
@@ -1152,16 +1152,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B18" t="s">
         <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E18" t="s">
         <v>27</v>
@@ -1169,13 +1169,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B19" t="s">
         <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D19" t="s">
         <v>5</v>
@@ -1186,13 +1186,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B20" t="s">
         <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D20" t="s">
         <v>30</v>
@@ -1203,13 +1203,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B21" t="s">
         <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D21" t="s">
         <v>5</v>
@@ -1220,13 +1220,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B22" t="s">
         <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D22" t="s">
         <v>12</v>
@@ -1237,24 +1237,24 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B23" t="s">
         <v>11</v>
       </c>
       <c r="C23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D23" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E23" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B24" t="s">
         <v>36</v>
@@ -1271,13 +1271,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B25" t="s">
         <v>39</v>
       </c>
       <c r="C25" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D25" t="s">
         <v>5</v>
@@ -1305,16 +1305,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B27" t="s">
         <v>44</v>
       </c>
       <c r="C27" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E27" t="s">
         <v>45</v>
@@ -1322,36 +1322,36 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B28" t="s">
         <v>11</v>
       </c>
       <c r="C28" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D28" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E28" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B29" t="s">
         <v>46</v>
       </c>
       <c r="C29" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D29" t="s">
         <v>30</v>
       </c>
       <c r="E29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1362,10 +1362,10 @@
         <v>48</v>
       </c>
       <c r="C30" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E30" t="s">
         <v>49</v>
@@ -1373,30 +1373,30 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>148</v>
+      </c>
+      <c r="B31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" t="s">
+        <v>137</v>
+      </c>
+      <c r="D31" t="s">
+        <v>76</v>
+      </c>
+      <c r="E31" t="s">
         <v>64</v>
-      </c>
-      <c r="B31" t="s">
-        <v>65</v>
-      </c>
-      <c r="C31" t="s">
-        <v>140</v>
-      </c>
-      <c r="D31" t="s">
-        <v>78</v>
-      </c>
-      <c r="E31" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B32" t="s">
         <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D32" t="s">
         <v>16</v>
@@ -1407,13 +1407,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B33" t="s">
         <v>39</v>
       </c>
       <c r="C33" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D33" t="s">
         <v>30</v>
@@ -1424,30 +1424,30 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B34" t="s">
         <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="D34" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E34" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B35" t="s">
         <v>35</v>
       </c>
       <c r="C35" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D35" t="s">
         <v>5</v>
@@ -1458,33 +1458,33 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B36" t="s">
         <v>11</v>
       </c>
       <c r="C36" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D36" t="s">
         <v>5</v>
       </c>
       <c r="E36" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B37" t="s">
         <v>44</v>
       </c>
       <c r="C37" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D37" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E37" t="s">
         <v>53</v>
@@ -1492,30 +1492,30 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C38" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D38" t="s">
         <v>16</v>
       </c>
       <c r="E38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B39" t="s">
         <v>21</v>
       </c>
       <c r="C39" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D39" t="s">
         <v>5</v>
@@ -1526,36 +1526,36 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B40" t="s">
         <v>11</v>
       </c>
       <c r="C40" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D40" t="s">
         <v>5</v>
       </c>
       <c r="E40" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B41" t="s">
         <v>32</v>
       </c>
       <c r="C41" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D41" t="s">
         <v>5</v>
       </c>
       <c r="E41" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -1566,10 +1566,10 @@
         <v>11</v>
       </c>
       <c r="C42" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D42" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E42" t="s">
         <v>56</v>
@@ -1577,19 +1577,19 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B43" t="s">
         <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>57</v>
+        <v>147</v>
       </c>
       <c r="D43" t="s">
         <v>16</v>
       </c>
       <c r="E43" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected typo on Members list
</commit_message>
<xml_diff>
--- a/data/P2P_members_list.xlsx
+++ b/data/P2P_members_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enriquemontes/p2p/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65A2F9C-F910-2542-A70E-80BFADDF0074}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD88C80-8F43-6D48-A775-CC3A41A51FB0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="2840" windowWidth="33120" windowHeight="16600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -363,9 +363,6 @@
     <t>[Maritza Cardenas](https://oceanexpert.org/expert/30409){target="_blank"}</t>
   </si>
   <si>
-    <t>Melissa Miner{target="_blank"}</t>
-  </si>
-  <si>
     <t>[Nicolas Moity](https://oceanexpert.org/expert/29466){target="_blank"}</t>
   </si>
   <si>
@@ -511,6 +508,9 @@
   </si>
   <si>
     <t>marianna.lanari@gmail.com</t>
+  </si>
+  <si>
+    <t>Melissa Miner</t>
   </si>
 </sst>
 </file>
@@ -891,7 +891,7 @@
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -926,13 +926,13 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D2" t="s">
         <v>71</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -943,7 +943,7 @@
         <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -960,7 +960,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -977,7 +977,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
@@ -994,7 +994,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
@@ -1011,7 +1011,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
@@ -1028,7 +1028,7 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
@@ -1045,7 +1045,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
@@ -1062,7 +1062,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D10" t="s">
         <v>16</v>
@@ -1079,7 +1079,7 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D11" t="s">
         <v>5</v>
@@ -1096,7 +1096,7 @@
         <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>
@@ -1113,7 +1113,7 @@
         <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D13" t="s">
         <v>16</v>
@@ -1141,19 +1141,19 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B15" t="s">
         <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D15" t="s">
         <v>72</v>
       </c>
       <c r="E15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1164,7 +1164,7 @@
         <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D16" t="s">
         <v>16</v>
@@ -1181,7 +1181,7 @@
         <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D17" t="s">
         <v>67</v>
@@ -1198,7 +1198,7 @@
         <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D18" t="s">
         <v>72</v>
@@ -1215,7 +1215,7 @@
         <v>11</v>
       </c>
       <c r="C19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D19" t="s">
         <v>73</v>
@@ -1232,7 +1232,7 @@
         <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D20" t="s">
         <v>5</v>
@@ -1249,7 +1249,7 @@
         <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D21" t="s">
         <v>59</v>
@@ -1266,7 +1266,7 @@
         <v>31</v>
       </c>
       <c r="C22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D22" t="s">
         <v>5</v>
@@ -1283,7 +1283,7 @@
         <v>11</v>
       </c>
       <c r="C23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D23" t="s">
         <v>12</v>
@@ -1300,7 +1300,7 @@
         <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D24" t="s">
         <v>77</v>
@@ -1317,7 +1317,7 @@
         <v>35</v>
       </c>
       <c r="C25" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D25" t="s">
         <v>5</v>
@@ -1334,7 +1334,7 @@
         <v>37</v>
       </c>
       <c r="C26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D26" t="s">
         <v>5</v>
@@ -1351,7 +1351,7 @@
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D27" t="s">
         <v>16</v>
@@ -1368,7 +1368,7 @@
         <v>41</v>
       </c>
       <c r="C28" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D28" t="s">
         <v>59</v>
@@ -1385,7 +1385,7 @@
         <v>11</v>
       </c>
       <c r="C29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D29" t="s">
         <v>72</v>
@@ -1396,19 +1396,19 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B30" t="s">
         <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D30" t="s">
         <v>59</v>
       </c>
       <c r="E30" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -1419,7 +1419,7 @@
         <v>43</v>
       </c>
       <c r="C31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D31" t="s">
         <v>59</v>
@@ -1436,7 +1436,7 @@
         <v>45</v>
       </c>
       <c r="C32" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D32" t="s">
         <v>59</v>
@@ -1453,7 +1453,7 @@
         <v>60</v>
       </c>
       <c r="C33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D33" t="s">
         <v>73</v>
@@ -1470,7 +1470,7 @@
         <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D34" t="s">
         <v>16</v>
@@ -1481,19 +1481,19 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B35" t="s">
         <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D35" t="s">
         <v>72</v>
       </c>
       <c r="E35" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -1504,7 +1504,7 @@
         <v>37</v>
       </c>
       <c r="C36" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D36" t="s">
         <v>59</v>
@@ -1521,7 +1521,7 @@
         <v>11</v>
       </c>
       <c r="C37" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D37" t="s">
         <v>73</v>
@@ -1532,19 +1532,19 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B38" t="s">
         <v>4</v>
       </c>
       <c r="C38" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D38" t="s">
+        <v>156</v>
+      </c>
+      <c r="E38" t="s">
         <v>157</v>
-      </c>
-      <c r="E38" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -1555,7 +1555,7 @@
         <v>34</v>
       </c>
       <c r="C39" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D39" t="s">
         <v>5</v>
@@ -1566,13 +1566,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>109</v>
+        <v>158</v>
       </c>
       <c r="B40" t="s">
         <v>11</v>
       </c>
       <c r="C40" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D40" t="s">
         <v>5</v>
@@ -1583,13 +1583,13 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B41" t="s">
         <v>41</v>
       </c>
       <c r="C41" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D41" t="s">
         <v>59</v>
@@ -1600,13 +1600,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B42" t="s">
         <v>56</v>
       </c>
       <c r="C42" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D42" t="s">
         <v>16</v>
@@ -1617,13 +1617,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B43" t="s">
         <v>21</v>
       </c>
       <c r="C43" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D43" t="s">
         <v>5</v>
@@ -1640,7 +1640,7 @@
         <v>11</v>
       </c>
       <c r="C44" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D44" t="s">
         <v>5</v>
@@ -1651,13 +1651,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B45" t="s">
         <v>31</v>
       </c>
       <c r="C45" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D45" t="s">
         <v>5</v>
@@ -1674,7 +1674,7 @@
         <v>11</v>
       </c>
       <c r="C46" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D46" t="s">
         <v>72</v>
@@ -1685,13 +1685,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B47" t="s">
         <v>4</v>
       </c>
       <c r="C47" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D47" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
+ new sites in Canada
</commit_message>
<xml_diff>
--- a/data/P2P_members_list.xlsx
+++ b/data/P2P_members_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10808"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enriquemontes/p2p/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD88C80-8F43-6D48-A775-CC3A41A51FB0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4285B92C-BA97-E848-B849-0F4664AA179F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="2840" windowWidth="33120" windowHeight="16600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="162">
   <si>
     <t>Country</t>
   </si>
@@ -511,6 +511,15 @@
   </si>
   <si>
     <t>Melissa Miner</t>
+  </si>
+  <si>
+    <t>Bethany Reinhart</t>
+  </si>
+  <si>
+    <t>[Fisheries and Ocean Canada](https://www.mar.dfo-mpo.gc.ca/SABS/Home)</t>
+  </si>
+  <si>
+    <t>bethany.reinhart@dfo-mpo.gc.ca</t>
   </si>
 </sst>
 </file>
@@ -888,10 +897,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1039,664 +1048,681 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>85</v>
+        <v>159</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="D9" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>85</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D11" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>124</v>
       </c>
       <c r="D14" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>153</v>
+        <v>89</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>149</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>72</v>
+        <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>154</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>90</v>
+        <v>153</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>125</v>
+        <v>149</v>
       </c>
       <c r="D16" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="E16" t="s">
-        <v>25</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D17" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="C18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D18" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E18" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B19" t="s">
         <v>11</v>
       </c>
       <c r="C19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D20" t="s">
-        <v>5</v>
+        <v>73</v>
       </c>
       <c r="E20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B21" t="s">
         <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D21" t="s">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="E21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D22" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="E22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="C23" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D23" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B24" t="s">
         <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D24" t="s">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="E24" t="s">
-        <v>78</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D25" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="E25" t="s">
-        <v>36</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B26" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D26" t="s">
         <v>5</v>
       </c>
       <c r="E26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>100</v>
       </c>
       <c r="B27" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="C27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D27" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="E27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>101</v>
+        <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D28" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="E28" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B29" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="C29" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="D29" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="E29" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>148</v>
+        <v>102</v>
       </c>
       <c r="B30" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C30" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="D30" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="E30" t="s">
-        <v>150</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>103</v>
+        <v>148</v>
       </c>
       <c r="B31" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="D31" t="s">
         <v>59</v>
       </c>
       <c r="E31" t="s">
-        <v>70</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>44</v>
+        <v>103</v>
       </c>
       <c r="B32" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C32" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D32" t="s">
         <v>59</v>
       </c>
       <c r="E32" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>104</v>
+        <v>44</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C33" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D33" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="E33" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B34" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="C34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D34" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="E34" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>152</v>
+        <v>105</v>
       </c>
       <c r="B35" t="s">
         <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="D35" t="s">
-        <v>72</v>
+        <v>16</v>
       </c>
       <c r="E35" t="s">
-        <v>151</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>106</v>
+        <v>152</v>
       </c>
       <c r="B36" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="D36" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="E36" t="s">
-        <v>48</v>
+        <v>151</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B37" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="C37" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D37" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="E37" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>155</v>
+        <v>107</v>
       </c>
       <c r="B38" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D38" t="s">
-        <v>156</v>
+        <v>73</v>
       </c>
       <c r="E38" t="s">
-        <v>157</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>108</v>
+        <v>155</v>
       </c>
       <c r="B39" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="D39" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="E39" t="s">
-        <v>49</v>
+        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>158</v>
+        <v>108</v>
       </c>
       <c r="B40" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="C40" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D40" t="s">
         <v>5</v>
       </c>
       <c r="E40" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>109</v>
+        <v>158</v>
       </c>
       <c r="B41" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="C41" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D41" t="s">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="E41" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B42" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="D42" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="E42" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B43" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="C43" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="D43" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E43" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>75</v>
+        <v>111</v>
       </c>
       <c r="B44" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C44" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D44" t="s">
         <v>5</v>
       </c>
       <c r="E44" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="B45" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="C45" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="D45" t="s">
         <v>5</v>
       </c>
       <c r="E45" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>52</v>
+        <v>112</v>
       </c>
       <c r="B46" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="C46" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D46" t="s">
-        <v>72</v>
+        <v>5</v>
       </c>
       <c r="E46" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" t="s">
+        <v>138</v>
+      </c>
+      <c r="D47" t="s">
+        <v>72</v>
+      </c>
+      <c r="E47" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>113</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>4</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>146</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D48" t="s">
         <v>16</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E48" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed affiliation of S. Habtes
</commit_message>
<xml_diff>
--- a/data/P2P_members_list.xlsx
+++ b/data/P2P_members_list.xlsx
@@ -1,31 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20377"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enriquemontes/p2p/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enrique\Documents\p2p\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4285B92C-BA97-E848-B849-0F4664AA179F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E760E328-C4F8-4B41-9596-640D7D40B15D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="2840" windowWidth="33120" windowHeight="16600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="2835" windowWidth="33120" windowHeight="16605" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P2P_members" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -34,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="164">
   <si>
     <t>Country</t>
   </si>
@@ -195,9 +186,6 @@
     <t>Sennai Habtes</t>
   </si>
   <si>
-    <t>sennai.habtes@uvi.edu</t>
-  </si>
-  <si>
     <t>yasmina.shahesmaeili@gmail.com</t>
   </si>
   <si>
@@ -520,6 +508,15 @@
   </si>
   <si>
     <t>bethany.reinhart@dfo-mpo.gc.ca</t>
+  </si>
+  <si>
+    <t>[USVI Dept. Planning &amp; Natural Resources](https://dpnr.vi.gov/fish-and-wildlife/){target="_blank"}</t>
+  </si>
+  <si>
+    <t>sennai.habtes@dpnr.vi.gov</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bureau Chief of Fisheries </t>
   </si>
 </sst>
 </file>
@@ -899,20 +896,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -927,49 +924,49 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
       <c r="C2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
         <v>114</v>
-      </c>
-      <c r="D2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" t="s">
-        <v>115</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -978,15 +975,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
@@ -995,15 +992,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
@@ -1012,15 +1009,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
@@ -1029,15 +1026,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
@@ -1046,32 +1043,32 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="s">
+        <v>159</v>
+      </c>
+      <c r="D9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" t="s">
         <v>160</v>
       </c>
-      <c r="D9" t="s">
-        <v>59</v>
-      </c>
-      <c r="E9" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D10" t="s">
         <v>5</v>
@@ -1080,7 +1077,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1088,7 +1085,7 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D11" t="s">
         <v>16</v>
@@ -1097,15 +1094,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>
@@ -1114,15 +1111,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B13" t="s">
         <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -1131,26 +1128,26 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
       </c>
       <c r="E14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B15" t="s">
         <v>21</v>
@@ -1165,32 +1162,32 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B16" t="s">
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E16" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B17" t="s">
         <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D17" t="s">
         <v>16</v>
@@ -1199,66 +1196,66 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" t="s">
+        <v>125</v>
+      </c>
+      <c r="D18" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>91</v>
-      </c>
-      <c r="B18" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" t="s">
-        <v>126</v>
-      </c>
-      <c r="D18" t="s">
-        <v>67</v>
-      </c>
-      <c r="E18" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>92</v>
       </c>
       <c r="B19" t="s">
         <v>11</v>
       </c>
       <c r="C19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E20" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B21" t="s">
         <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D21" t="s">
         <v>5</v>
@@ -1267,32 +1264,32 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B22" t="s">
         <v>28</v>
       </c>
       <c r="C22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E22" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B23" t="s">
         <v>31</v>
       </c>
       <c r="C23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D23" t="s">
         <v>5</v>
@@ -1301,15 +1298,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B24" t="s">
         <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D24" t="s">
         <v>12</v>
@@ -1318,32 +1315,32 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B25" t="s">
         <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D25" t="s">
+        <v>76</v>
+      </c>
+      <c r="E25" t="s">
         <v>77</v>
       </c>
-      <c r="E25" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B26" t="s">
         <v>35</v>
       </c>
       <c r="C26" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D26" t="s">
         <v>5</v>
@@ -1352,15 +1349,15 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B27" t="s">
         <v>37</v>
       </c>
       <c r="C27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D27" t="s">
         <v>5</v>
@@ -1369,7 +1366,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -1377,7 +1374,7 @@
         <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D28" t="s">
         <v>16</v>
@@ -1386,75 +1383,75 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B29" t="s">
         <v>41</v>
       </c>
       <c r="C29" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E29" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B30" t="s">
         <v>11</v>
       </c>
       <c r="C30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B31" t="s">
         <v>4</v>
       </c>
       <c r="C31" t="s">
+        <v>148</v>
+      </c>
+      <c r="D31" t="s">
+        <v>58</v>
+      </c>
+      <c r="E31" t="s">
         <v>149</v>
       </c>
-      <c r="D31" t="s">
-        <v>59</v>
-      </c>
-      <c r="E31" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B32" t="s">
         <v>43</v>
       </c>
       <c r="C32" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E32" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -1462,41 +1459,41 @@
         <v>45</v>
       </c>
       <c r="C33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E33" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>103</v>
+      </c>
+      <c r="B34" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" t="s">
+        <v>138</v>
+      </c>
+      <c r="D34" t="s">
+        <v>72</v>
+      </c>
+      <c r="E34" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>104</v>
-      </c>
-      <c r="B34" t="s">
-        <v>60</v>
-      </c>
-      <c r="C34" t="s">
-        <v>139</v>
-      </c>
-      <c r="D34" t="s">
-        <v>73</v>
-      </c>
-      <c r="E34" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>105</v>
       </c>
       <c r="B35" t="s">
         <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D35" t="s">
         <v>16</v>
@@ -1505,83 +1502,83 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B36" t="s">
         <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D36" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E36" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B37" t="s">
         <v>37</v>
       </c>
       <c r="C37" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E37" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B38" t="s">
         <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E38" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B39" t="s">
         <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D39" t="s">
+        <v>155</v>
+      </c>
+      <c r="E39" t="s">
         <v>156</v>
       </c>
-      <c r="E39" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B40" t="s">
         <v>34</v>
       </c>
       <c r="C40" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D40" t="s">
         <v>5</v>
@@ -1590,66 +1587,66 @@
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B41" t="s">
         <v>11</v>
       </c>
       <c r="C41" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D41" t="s">
         <v>5</v>
       </c>
       <c r="E41" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B42" t="s">
         <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D42" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C43" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D43" t="s">
         <v>16</v>
       </c>
       <c r="E43" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B44" t="s">
         <v>21</v>
       </c>
       <c r="C44" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D44" t="s">
         <v>5</v>
@@ -1658,41 +1655,41 @@
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B45" t="s">
         <v>11</v>
       </c>
       <c r="C45" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D45" t="s">
         <v>5</v>
       </c>
       <c r="E45" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B46" t="s">
         <v>31</v>
       </c>
       <c r="C46" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D46" t="s">
         <v>5</v>
       </c>
       <c r="E46" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -1700,33 +1697,36 @@
         <v>11</v>
       </c>
       <c r="C47" t="s">
-        <v>138</v>
+        <v>161</v>
       </c>
       <c r="D47" t="s">
-        <v>72</v>
+        <v>163</v>
       </c>
       <c r="E47" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B48" t="s">
         <v>4</v>
       </c>
       <c r="C48" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D48" t="s">
         <v>16</v>
       </c>
       <c r="E48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E47" r:id="rId1" xr:uid="{249375E2-EDD7-4DDC-B62E-FE3D76DCC9C0}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Added Sergio Cerdeira to the Members list
</commit_message>
<xml_diff>
--- a/data/P2P_members_list.xlsx
+++ b/data/P2P_members_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20377"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11010"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enrique\Documents\p2p\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enriquemontes/p2p/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E760E328-C4F8-4B41-9596-640D7D40B15D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B11E4C9D-FD23-F544-AC00-E4CFD8E5B45E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="2835" windowWidth="33120" windowHeight="16605" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="340" yWindow="2840" windowWidth="33120" windowHeight="16600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P2P_members" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="167">
   <si>
     <t>Country</t>
   </si>
@@ -517,6 +517,15 @@
   </si>
   <si>
     <t xml:space="preserve">Bureau Chief of Fisheries </t>
+  </si>
+  <si>
+    <t>[Sergio Cerdeira](https://oceanexpert.org/expert/30635)</t>
+  </si>
+  <si>
+    <t>[CONABIO - SIMAR](https://simar.conabio.gob.mx/)</t>
+  </si>
+  <si>
+    <t>scerdeira@conabio.gob.mx</t>
   </si>
 </sst>
 </file>
@@ -894,20 +903,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="55.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -924,7 +933,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>78</v>
       </c>
@@ -941,7 +950,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -958,7 +967,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>79</v>
       </c>
@@ -975,7 +984,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>80</v>
       </c>
@@ -992,7 +1001,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>81</v>
       </c>
@@ -1009,7 +1018,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>82</v>
       </c>
@@ -1026,7 +1035,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>83</v>
       </c>
@@ -1043,7 +1052,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>158</v>
       </c>
@@ -1060,7 +1069,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>84</v>
       </c>
@@ -1077,7 +1086,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1094,7 +1103,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>85</v>
       </c>
@@ -1111,7 +1120,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>86</v>
       </c>
@@ -1128,7 +1137,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>87</v>
       </c>
@@ -1145,7 +1154,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>88</v>
       </c>
@@ -1162,7 +1171,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>152</v>
       </c>
@@ -1179,7 +1188,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>89</v>
       </c>
@@ -1196,7 +1205,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>90</v>
       </c>
@@ -1213,7 +1222,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>91</v>
       </c>
@@ -1230,7 +1239,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>92</v>
       </c>
@@ -1247,7 +1256,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>93</v>
       </c>
@@ -1264,7 +1273,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>94</v>
       </c>
@@ -1281,7 +1290,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>95</v>
       </c>
@@ -1298,7 +1307,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>96</v>
       </c>
@@ -1315,7 +1324,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>97</v>
       </c>
@@ -1332,7 +1341,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>98</v>
       </c>
@@ -1349,7 +1358,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>99</v>
       </c>
@@ -1366,7 +1375,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -1383,7 +1392,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>100</v>
       </c>
@@ -1400,7 +1409,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>101</v>
       </c>
@@ -1417,7 +1426,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>147</v>
       </c>
@@ -1434,7 +1443,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>102</v>
       </c>
@@ -1451,7 +1460,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -1468,7 +1477,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>103</v>
       </c>
@@ -1485,7 +1494,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>104</v>
       </c>
@@ -1502,7 +1511,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>151</v>
       </c>
@@ -1519,7 +1528,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>105</v>
       </c>
@@ -1536,7 +1545,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>106</v>
       </c>
@@ -1553,7 +1562,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>154</v>
       </c>
@@ -1570,7 +1579,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>107</v>
       </c>
@@ -1587,7 +1596,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>157</v>
       </c>
@@ -1604,7 +1613,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>108</v>
       </c>
@@ -1621,7 +1630,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>109</v>
       </c>
@@ -1638,7 +1647,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>110</v>
       </c>
@@ -1655,7 +1664,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>74</v>
       </c>
@@ -1672,7 +1681,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>111</v>
       </c>
@@ -1689,7 +1698,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -1706,20 +1715,37 @@
         <v>162</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>164</v>
+      </c>
+      <c r="B48" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" t="s">
+        <v>165</v>
+      </c>
+      <c r="D48" t="s">
+        <v>5</v>
+      </c>
+      <c r="E48" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>112</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>4</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>145</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D49" t="s">
         <v>16</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E49" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>